<commit_message>
add data files saved in revision
</commit_message>
<xml_diff>
--- a/Mason_SoilMicrobe-PMI_XXXXX_2023/data/MAE_tax-marker_anova.xlsx
+++ b/Mason_SoilMicrobe-PMI_XXXXX_2023/data/MAE_tax-marker_anova.xlsx
@@ -389,16 +389,16 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>21200.80112173162</v>
+        <v>21200.80112173163</v>
       </c>
       <c r="C2">
-        <v>10600.40056086581</v>
+        <v>10600.40056086582</v>
       </c>
       <c r="D2">
-        <v>9.65458907504277</v>
+        <v>9.654589075042781</v>
       </c>
       <c r="E2">
-        <v>0.001063068347309052</v>
+        <v>0.001063068347309045</v>
       </c>
     </row>
     <row r="3">
@@ -406,7 +406,7 @@
         <v>21</v>
       </c>
       <c r="B3">
-        <v>23057.26427586934</v>
+        <v>23057.26427586932</v>
       </c>
       <c r="C3">
         <v>1097.964965517587</v>

</xml_diff>